<commit_message>
Update .gitignore, EnoncéP8.jpg, and 19 more files...
</commit_message>
<xml_diff>
--- a/Ressources/Avancement.xlsx
+++ b/Ressources/Avancement.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjetOC_Seb\Projet_8\Ressources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenClassroom_projet\Projet_8\Ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47460423-F9BF-4B40-B681-096A1DDE7190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC61116-CD24-46AC-9FD7-84056124F901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t xml:space="preserve">Tache à réaliser : </t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>à optimiser encore</t>
+  </si>
+  <si>
+    <t>SVM -&gt; Unet -&gt; Mask_RCNN</t>
   </si>
 </sst>
 </file>
@@ -786,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -821,7 +824,7 @@
       <c r="D4" s="7"/>
       <c r="F4" s="3">
         <f>AVERAGE(C5:C10,C12:C17,C19:C21,C23:C25)</f>
-        <v>0.48888888888888893</v>
+        <v>0.51944444444444438</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -862,9 +865,11 @@
         <v>8</v>
       </c>
       <c r="C8" s="14">
-        <v>0.2</v>
-      </c>
-      <c r="D8" s="20"/>
+        <v>0.6</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="9" spans="2:7" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="20" t="s">
@@ -907,7 +912,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="12">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="D13" s="6"/>
       <c r="G13" s="19"/>

</xml_diff>

<commit_message>
Comparative modeling analysis, done Technical note write, done benchmark model and data generator, read file, done. flask application (to send on Azure) done.
</commit_message>
<xml_diff>
--- a/Ressources/Avancement.xlsx
+++ b/Ressources/Avancement.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenClassroom_projet\Projet_8\Ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC61116-CD24-46AC-9FD7-84056124F901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8CAE49E-1DB0-4C90-BDDC-31DE4D4EF5F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t xml:space="preserve">Tache à réaliser : </t>
   </si>
@@ -117,28 +117,16 @@
     <t>le script du générateur de données est entièrement automatisé</t>
   </si>
   <si>
-    <t>Label_id file</t>
-  </si>
-  <si>
-    <t>Oui mais pas utilisé encore</t>
-  </si>
-  <si>
-    <t>Idem</t>
-  </si>
-  <si>
-    <t>A implémenté</t>
-  </si>
-  <si>
-    <t>à vérifier</t>
-  </si>
-  <si>
-    <t>à tester plusieur approche et à synthétiser</t>
-  </si>
-  <si>
-    <t>à optimiser encore</t>
-  </si>
-  <si>
-    <t>SVM -&gt; Unet -&gt; Mask_RCNN</t>
+    <t>Le temps de calcul</t>
+  </si>
+  <si>
+    <t>SVM -&gt; Unet -&gt; FPN ?</t>
+  </si>
+  <si>
+    <t>MeanIoU / Temps</t>
+  </si>
+  <si>
+    <t>Via Azure CLI</t>
   </si>
 </sst>
 </file>
@@ -420,7 +408,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -447,9 +435,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -480,6 +465,12 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -789,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -817,132 +808,128 @@
       </c>
     </row>
     <row r="4" spans="2:7" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="27"/>
+      <c r="C4" s="28"/>
       <c r="D4" s="7"/>
       <c r="F4" s="3">
         <f>AVERAGE(C5:C10,C12:C17,C19:C21,C23:C25)</f>
-        <v>0.51944444444444438</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="12">
-        <v>1</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>27</v>
-      </c>
+      <c r="C5" s="11">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" spans="2:7" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="12">
-        <v>1</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>28</v>
-      </c>
+      <c r="C6" s="11">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5"/>
     </row>
     <row r="7" spans="2:7" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="13">
-        <v>1</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>29</v>
-      </c>
+      <c r="C7" s="12">
+        <v>1</v>
+      </c>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" spans="2:7" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="14">
-        <v>0.6</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>34</v>
+      <c r="C8" s="13">
+        <v>1</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="14">
-        <v>0</v>
-      </c>
-      <c r="D9" s="20"/>
+      <c r="C9" s="13">
+        <v>1</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="10" spans="2:7" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="D10" s="10"/>
+      <c r="C10" s="13">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5"/>
     </row>
     <row r="11" spans="2:7" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="25"/>
+      <c r="C11" s="26"/>
       <c r="D11" s="7"/>
     </row>
     <row r="12" spans="2:7" ht="82" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>30</v>
-      </c>
+      <c r="C12" s="11">
+        <v>1</v>
+      </c>
+      <c r="D12" s="6"/>
     </row>
     <row r="13" spans="2:7" ht="100" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="D13" s="6"/>
-      <c r="G13" s="19"/>
+      <c r="C13" s="11">
+        <v>1</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="2:7" ht="78.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="12">
-        <v>0</v>
-      </c>
-      <c r="D14" s="6"/>
+      <c r="C14" s="11">
+        <v>1</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="15" spans="2:7" ht="80.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>30</v>
-      </c>
+      <c r="C15" s="11">
+        <v>1</v>
+      </c>
+      <c r="D15" s="21"/>
     </row>
     <row r="16" spans="2:7" ht="83" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="12">
-        <v>0</v>
+      <c r="C16" s="11">
+        <v>1</v>
       </c>
       <c r="D16" s="6"/>
     </row>
@@ -950,26 +937,28 @@
       <c r="B17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="13">
-        <v>0</v>
-      </c>
-      <c r="D17" s="4"/>
+      <c r="C17" s="12">
+        <v>1</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="F17" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="77" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="23"/>
+      <c r="C18" s="24"/>
       <c r="D18" s="7"/>
     </row>
     <row r="19" spans="2:6" ht="79" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="11">
         <v>1</v>
       </c>
       <c r="D19" s="6"/>
@@ -978,47 +967,41 @@
       <c r="B20" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>31</v>
-      </c>
+      <c r="C20" s="11">
+        <v>1</v>
+      </c>
+      <c r="D20" s="21"/>
     </row>
     <row r="21" spans="2:6" ht="76" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B21" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="C21" s="12">
+        <v>1</v>
+      </c>
+      <c r="D21" s="4"/>
     </row>
     <row r="22" spans="2:6" ht="62.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="29"/>
-      <c r="D22" s="18"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="17"/>
     </row>
     <row r="23" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="16">
-        <v>1</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>33</v>
-      </c>
+      <c r="C23" s="15">
+        <v>1</v>
+      </c>
+      <c r="D23" s="22"/>
     </row>
     <row r="24" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="21">
+      <c r="C24" s="20">
         <v>1</v>
       </c>
       <c r="D24" s="6"/>
@@ -1027,10 +1010,10 @@
       <c r="B25" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="17">
-        <v>1</v>
-      </c>
-      <c r="D25" s="4"/>
+      <c r="C25" s="16">
+        <v>1</v>
+      </c>
+      <c r="D25" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>